<commit_message>
Update causal inference module after Fall 2022 class
This commit contains changes that reflect the state of the module at the end of the Fall 2022 class period.
</commit_message>
<xml_diff>
--- a/modules/04 Measures of Association/Examples for understand the Szklo Text - Measures of Association.xlsx
+++ b/modules/04 Measures of Association/Examples for understand the Szklo Text - Measures of Association.xlsx
@@ -4618,8 +4618,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED41D9ADB7F09344BC6B7E44F29CCBFD" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95f2ade63b6a87fda67820bb1fb1aefa">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e3793ca1-6164-4dfb-aaf8-0aa60c0c70c2" xmlns:ns3="b3558f30-ae73-4668-947b-5578bd4f9b3c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e10a55ace02b924c5615230c40e2e4e5" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED41D9ADB7F09344BC6B7E44F29CCBFD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8758a9079f5c81cc9bbaf8817f1682cc">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e3793ca1-6164-4dfb-aaf8-0aa60c0c70c2" xmlns:ns3="b3558f30-ae73-4668-947b-5578bd4f9b3c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f4c82a11dbf66c51fd0803d992e2d3ac" ns2:_="" ns3:_="">
     <xsd:import namespace="e3793ca1-6164-4dfb-aaf8-0aa60c0c70c2"/>
     <xsd:import namespace="b3558f30-ae73-4668-947b-5578bd4f9b3c"/>
     <xsd:element name="properties">
@@ -4638,6 +4638,8 @@
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -4711,6 +4713,32 @@
           </xsd:extension>
         </xsd:complexContent>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -4833,7 +4861,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4589FAB3-9819-4C74-9761-0E1C7495EE1B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0AF0566-2425-4AA7-AA21-26EA0FAE3C9A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>